<commit_message>
Compile codegen fixes #
</commit_message>
<xml_diff>
--- a/CodeGenerators/out/parsed.xlsx
+++ b/CodeGenerators/out/parsed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="167">
   <si>
     <t>ROW</t>
   </si>
@@ -34,27 +34,21 @@
     <t>PICK</t>
   </si>
   <si>
+    <t>DATE</t>
+  </si>
+  <si>
     <t>TXT</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>CQ1</t>
   </si>
   <si>
     <t>CQ2</t>
   </si>
   <si>
-    <t>CQ2.1</t>
-  </si>
-  <si>
     <t>CQ3</t>
   </si>
   <si>
-    <t>CQ3.1</t>
-  </si>
-  <si>
     <t>CQ4</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>CQ4b</t>
   </si>
   <si>
-    <t>CQ4b.1</t>
-  </si>
-  <si>
     <t>CQ4c</t>
   </si>
   <si>
@@ -94,15 +85,6 @@
     <t>CQ7a</t>
   </si>
   <si>
-    <t>CQ7a.1</t>
-  </si>
-  <si>
-    <t>CQ5.1</t>
-  </si>
-  <si>
-    <t>CQ7.1</t>
-  </si>
-  <si>
     <t>CQ7b</t>
   </si>
   <si>
@@ -121,9 +103,6 @@
     <t>CQ11</t>
   </si>
   <si>
-    <t>CQ11.1</t>
-  </si>
-  <si>
     <t>CQ12</t>
   </si>
   <si>
@@ -199,9 +178,6 @@
     <t>CQ27</t>
   </si>
   <si>
-    <t>CQ27.1</t>
-  </si>
-  <si>
     <t>CQ28</t>
   </si>
   <si>
@@ -211,9 +187,6 @@
     <t>CQ29A</t>
   </si>
   <si>
-    <t>CQ29A.1</t>
-  </si>
-  <si>
     <t>CQ29B</t>
   </si>
   <si>
@@ -296,9 +269,6 @@
   </si>
   <si>
     <t>What services does the HVA system provide? Please select all that apply.</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>To whom does the HVA provide services to? Please select all that apply.</t>
@@ -903,7 +873,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -937,7 +907,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>356</v>
@@ -954,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -965,16 +935,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -985,13 +955,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -999,16 +969,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E6">
-        <v>355</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1019,13 +989,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E7">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1039,7 +1009,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E8">
         <v>162</v>
@@ -1056,10 +1026,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>326</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1073,10 +1043,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1090,10 +1060,10 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1107,7 +1077,7 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E12">
         <v>162</v>
@@ -1118,16 +1088,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E13">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1135,16 +1105,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1158,7 +1128,7 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E15">
         <v>162</v>
@@ -1169,16 +1139,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1192,10 +1162,10 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E17">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1206,10 +1176,10 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E18">
         <v>162</v>
@@ -1220,16 +1190,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E19">
-        <v>153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1240,10 +1210,10 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1254,16 +1224,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E21">
-        <v>154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1274,13 +1244,13 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1288,16 +1258,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E23">
-        <v>162</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1305,16 +1275,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1325,13 +1295,13 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1342,13 +1312,13 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1359,13 +1329,13 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E27">
-        <v>327</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1373,16 +1343,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E28">
-        <v>328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1390,16 +1360,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1407,16 +1377,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E30">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1424,16 +1394,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E31">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1441,16 +1411,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E32">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1464,10 +1434,10 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E33">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1475,13 +1445,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1492,16 +1462,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1515,10 +1485,10 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E36">
-        <v>155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1526,13 +1496,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1543,13 +1513,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1560,16 +1530,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1583,7 +1553,7 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E40">
         <v>162</v>
@@ -1594,16 +1564,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1611,16 +1581,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E42">
-        <v>156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1634,10 +1604,10 @@
         <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1645,13 +1615,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
         <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1668,7 +1638,7 @@
         <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1685,10 +1655,10 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E46">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1702,10 +1672,10 @@
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E47">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1719,7 +1689,7 @@
         <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E48">
         <v>162</v>
@@ -1730,13 +1700,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1753,10 +1723,10 @@
         <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E50">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1764,16 +1734,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
         <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1787,7 +1757,7 @@
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1798,13 +1768,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1821,7 +1791,7 @@
         <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1838,10 +1808,10 @@
         <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E55">
-        <v>162</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1849,16 +1819,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1872,10 +1842,10 @@
         <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1889,10 +1859,10 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E58">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1906,10 +1876,10 @@
         <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1917,16 +1887,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1940,10 +1910,10 @@
         <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1957,10 +1927,10 @@
         <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E62">
-        <v>362</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1974,10 +1944,10 @@
         <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E63">
-        <v>6</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1985,16 +1955,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
         <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="E64">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2008,10 +1978,10 @@
         <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E65">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2025,10 +1995,10 @@
         <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2042,10 +2012,10 @@
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2053,13 +2023,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
         <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="E68">
         <v>157</v>
@@ -2076,7 +2046,7 @@
         <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E69">
         <v>157</v>
@@ -2087,16 +2057,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E70">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2107,13 +2077,13 @@
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E71">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2121,16 +2091,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E72">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2138,16 +2108,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D73" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E73">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2158,13 +2128,13 @@
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E74">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2175,13 +2145,13 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E75">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2192,13 +2162,13 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E76">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2209,13 +2179,13 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E77">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2226,13 +2196,13 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E78">
-        <v>157</v>
+        <v>329</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2240,13 +2210,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2257,16 +2227,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
         <v>76</v>
       </c>
       <c r="D80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E80">
-        <v>158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2274,13 +2244,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
         <v>77</v>
       </c>
       <c r="D81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2291,13 +2261,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
         <v>78</v>
       </c>
       <c r="D82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2314,7 +2284,7 @@
         <v>79</v>
       </c>
       <c r="D83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E83">
         <v>162</v>
@@ -2331,7 +2301,7 @@
         <v>80</v>
       </c>
       <c r="D84" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E84">
         <v>162</v>
@@ -2348,7 +2318,7 @@
         <v>81</v>
       </c>
       <c r="D85" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E85">
         <v>162</v>
@@ -2365,162 +2335,9 @@
         <v>82</v>
       </c>
       <c r="D86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E86">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" t="s">
-        <v>83</v>
-      </c>
-      <c r="D87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E87">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" t="s">
-        <v>84</v>
-      </c>
-      <c r="D88" t="s">
-        <v>170</v>
-      </c>
-      <c r="E88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>85</v>
-      </c>
-      <c r="D89" t="s">
-        <v>171</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>86</v>
-      </c>
-      <c r="D90" t="s">
-        <v>172</v>
-      </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" t="s">
-        <v>87</v>
-      </c>
-      <c r="D91" t="s">
-        <v>173</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" t="s">
-        <v>88</v>
-      </c>
-      <c r="D92" t="s">
-        <v>174</v>
-      </c>
-      <c r="E92">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="B93" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" t="s">
-        <v>89</v>
-      </c>
-      <c r="D93" t="s">
-        <v>168</v>
-      </c>
-      <c r="E93">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="B94" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" t="s">
-        <v>90</v>
-      </c>
-      <c r="D94" t="s">
-        <v>175</v>
-      </c>
-      <c r="E94">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" t="s">
-        <v>91</v>
-      </c>
-      <c r="D95" t="s">
-        <v>176</v>
-      </c>
-      <c r="E95">
         <v>329</v>
       </c>
     </row>

</xml_diff>